<commit_message>
CP-272, CP-312, CP-313, CP-314: Created an Explicit Eligibility template to map Students to their Tests. Updated ART Test Selector so that it sets the Eligibility Type to Explicit. Created an Explicit Eligibility Uploader to upload the Explicit Eligibilities.
</commit_message>
<xml_diff>
--- a/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
   <si>
     <t>Test</t>
   </si>
@@ -99,24 +99,6 @@
     <t>AlternateSSID</t>
   </si>
   <si>
-    <t>A39990001</t>
-  </si>
-  <si>
-    <t>A39990002</t>
-  </si>
-  <si>
-    <t>A79990001</t>
-  </si>
-  <si>
-    <t>A79990002</t>
-  </si>
-  <si>
-    <t>A119990001</t>
-  </si>
-  <si>
-    <t>A119990002</t>
-  </si>
-  <si>
     <t>CAT</t>
   </si>
   <si>
@@ -202,6 +184,45 @@
   </si>
   <si>
     <t>Directions: Register each of the following students (Column F, G, H) with the corresponding test (Column A)</t>
+  </si>
+  <si>
+    <t>IRP39990001</t>
+  </si>
+  <si>
+    <t>IRP39990002</t>
+  </si>
+  <si>
+    <t>IRP79990001</t>
+  </si>
+  <si>
+    <t>IRP79990002</t>
+  </si>
+  <si>
+    <t>IRP119990001</t>
+  </si>
+  <si>
+    <t>IRP119990002</t>
+  </si>
+  <si>
+    <t>AIRP39990001</t>
+  </si>
+  <si>
+    <t>AIRP39990002</t>
+  </si>
+  <si>
+    <t>ARP39990002</t>
+  </si>
+  <si>
+    <t>AIRP79990001</t>
+  </si>
+  <si>
+    <t>AIRP79990002</t>
+  </si>
+  <si>
+    <t>AIRP119990001</t>
+  </si>
+  <si>
+    <t>AIRP119990002</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1137,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1158,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1152,16 +1173,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -1178,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1186,11 +1207,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>39990001</v>
+      <c r="F3" t="s">
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
@@ -1201,7 +1222,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1212,11 +1233,11 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>39990001</v>
+      <c r="F4" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
@@ -1227,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1235,11 +1256,11 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="F5">
-        <v>39990002</v>
+      <c r="F5" t="s">
+        <v>52</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>16</v>
@@ -1250,7 +1271,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1261,11 +1282,11 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>39990002</v>
+      <c r="F6" t="s">
+        <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>16</v>
@@ -1276,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1284,11 +1305,11 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="F7">
-        <v>79990001</v>
+      <c r="F7" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>17</v>
@@ -1299,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1310,11 +1331,11 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>79990001</v>
+      <c r="F8" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>17</v>
@@ -1325,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1333,11 +1354,11 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="F9">
-        <v>79990002</v>
+      <c r="F9" t="s">
+        <v>54</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>18</v>
@@ -1349,7 +1370,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1360,11 +1381,11 @@
       <c r="E10" t="b">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>79990002</v>
+      <c r="F10" t="s">
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>18</v>
@@ -1375,7 +1396,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1383,11 +1404,11 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>119990001</v>
+      <c r="F11" t="s">
+        <v>55</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>19</v>
@@ -1399,7 +1420,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1410,11 +1431,11 @@
       <c r="E12" t="b">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>119990001</v>
+      <c r="F12" t="s">
+        <v>55</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>19</v>
@@ -1425,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -1433,11 +1454,11 @@
       <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F13">
-        <v>119990002</v>
+      <c r="F13" t="s">
+        <v>56</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
@@ -1448,7 +1469,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1459,11 +1480,11 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>119990002</v>
+      <c r="F14" t="s">
+        <v>56</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>20</v>
@@ -1471,22 +1492,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>39990001</v>
+      <c r="F15" t="s">
+        <v>51</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>15</v>
@@ -1494,22 +1515,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>39990001</v>
+      <c r="F16" t="s">
+        <v>51</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
@@ -1517,13 +1538,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -1531,11 +1552,11 @@
       <c r="E17" t="b">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>39990001</v>
+      <c r="F17" t="s">
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>15</v>
@@ -1543,22 +1564,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F18">
-        <v>79990001</v>
+      <c r="F18" t="s">
+        <v>53</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>17</v>
@@ -1566,22 +1587,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F19">
-        <v>79990001</v>
+      <c r="F19" t="s">
+        <v>53</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>17</v>
@@ -1589,13 +1610,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1603,11 +1624,11 @@
       <c r="E20" t="b">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>79990001</v>
+      <c r="F20" t="s">
+        <v>53</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>17</v>
@@ -1615,22 +1636,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="F21">
-        <v>119990001</v>
+      <c r="F21" t="s">
+        <v>55</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
@@ -1638,22 +1659,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
-        <v>119990001</v>
+      <c r="F22" t="s">
+        <v>55</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>19</v>
@@ -1661,13 +1682,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1675,11 +1696,11 @@
       <c r="E23" t="b">
         <v>1</v>
       </c>
-      <c r="F23">
-        <v>119990001</v>
+      <c r="F23" t="s">
+        <v>55</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>19</v>
@@ -1687,22 +1708,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F24">
-        <v>39990002</v>
+      <c r="F24" t="s">
+        <v>52</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>16</v>
@@ -1710,13 +1731,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>4</v>
@@ -1724,11 +1745,11 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="F25">
-        <v>39990002</v>
+      <c r="F25" t="s">
+        <v>52</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>16</v>
@@ -1736,22 +1757,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="F26">
-        <v>79990002</v>
+      <c r="F26" t="s">
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>18</v>
@@ -1759,13 +1780,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1773,11 +1794,11 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27">
-        <v>79990002</v>
+      <c r="F27" t="s">
+        <v>54</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>18</v>
@@ -1785,13 +1806,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1799,11 +1820,11 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>79990002</v>
+      <c r="F28" t="s">
+        <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>18</v>
@@ -1811,22 +1832,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
-      <c r="F29">
-        <v>119990002</v>
+      <c r="F29" t="s">
+        <v>56</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>20</v>
@@ -1834,13 +1855,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -1848,11 +1869,11 @@
       <c r="E30" t="b">
         <v>1</v>
       </c>
-      <c r="F30">
-        <v>119990002</v>
+      <c r="F30" t="s">
+        <v>56</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
CP-159, CP-230: Using the Student to Test mapping CSV file, the StudentFactory creates all IRP Students to use for the simulation. They all take their tests synchronously.
</commit_message>
<xml_diff>
--- a/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="63">
   <si>
     <t>Test</t>
   </si>
@@ -78,24 +78,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>StudentA</t>
-  </si>
-  <si>
-    <t>StudentB</t>
-  </si>
-  <si>
-    <t>StudentC</t>
-  </si>
-  <si>
-    <t>StudentD</t>
-  </si>
-  <si>
-    <t>StudentE</t>
-  </si>
-  <si>
-    <t>StudentF</t>
-  </si>
-  <si>
     <t>AlternateSSID</t>
   </si>
   <si>
@@ -210,9 +192,6 @@
     <t>AIRP39990002</t>
   </si>
   <si>
-    <t>ARP39990002</t>
-  </si>
-  <si>
     <t>AIRP79990001</t>
   </si>
   <si>
@@ -223,6 +202,24 @@
   </si>
   <si>
     <t>AIRP119990002</t>
+  </si>
+  <si>
+    <t>IRPStudentA</t>
+  </si>
+  <si>
+    <t>IRPStudentB</t>
+  </si>
+  <si>
+    <t>IRPStudentC</t>
+  </si>
+  <si>
+    <t>IRPStudentD</t>
+  </si>
+  <si>
+    <t>IRPStudentE</t>
+  </si>
+  <si>
+    <t>IRPStudentF</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1158,7 +1155,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1173,22 +1170,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
@@ -1199,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1208,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1222,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1234,13 +1231,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1248,7 +1245,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1257,13 +1254,13 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1271,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1283,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1297,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1306,13 +1303,13 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1320,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1332,13 +1329,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1346,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1355,13 +1352,13 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="M9" s="6"/>
     </row>
@@ -1370,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1382,13 +1379,13 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1396,7 +1393,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1405,13 +1402,13 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="M11" s="7"/>
     </row>
@@ -1420,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1432,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1446,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -1455,13 +1452,13 @@
         <v>13</v>
       </c>
       <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1469,7 +1466,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1481,70 +1478,70 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -1553,70 +1550,70 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H18" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1625,70 +1622,70 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H22" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1697,47 +1694,47 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>4</v>
@@ -1746,47 +1743,47 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="F26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H26" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1795,24 +1792,24 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H27" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1821,47 +1818,47 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H28" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -1870,13 +1867,13 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H30" s="2" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>